<commit_message>
added missing techinque due to invalid mapping the initial file
</commit_message>
<xml_diff>
--- a/MiTRE/MitreOperations.xlsx
+++ b/MiTRE/MitreOperations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AssistantsTesterGithub\MiTRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFF8FC3-80A9-40D0-A05F-1D388BC0071C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C16F04-AACE-48DA-9CF7-BC5F199F3A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="279">
   <si>
     <t>Operation</t>
   </si>
@@ -507,24 +507,9 @@
     <t>ExecCount</t>
   </si>
   <si>
-    <t>Exec Operations</t>
-  </si>
-  <si>
-    <t>OldCount</t>
-  </si>
-  <si>
-    <t>NewCount</t>
-  </si>
-  <si>
     <t>T1003.002</t>
   </si>
   <si>
-    <t>ExecuteCount</t>
-  </si>
-  <si>
-    <t>OtherCount</t>
-  </si>
-  <si>
     <t>Open process + 2x Execute</t>
   </si>
   <si>
@@ -906,16 +891,10 @@
     <t>T1112</t>
   </si>
   <si>
-    <t>INTREB</t>
-  </si>
-  <si>
     <t>reg add HKCU\Software\Microsoft\Windows\CurrentVersion\Run /v MyApp /t REG_SZ /d "calc.exe" /f</t>
   </si>
   <si>
     <t>https://attack.mitre.org/techniques/T1112/</t>
-  </si>
-  <si>
-    <t>Pot rula orice comanda sau???</t>
   </si>
   <si>
     <r>
@@ -1155,6 +1134,9 @@
   </si>
   <si>
     <t>Approves</t>
+  </si>
+  <si>
+    <t>T1091.000.V1.cpp</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1233,12 +1215,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1264,13 +1240,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1282,9 +1255,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1568,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4627B1-CCD6-45EF-95C0-ACBE31171D5D}">
-  <dimension ref="A1:P130"/>
+  <dimension ref="A1:P131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,70 +1554,41 @@
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="44.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="3" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" customWidth="1"/>
     <col min="17" max="17" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="J1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <f>C2+D2*P2</f>
-        <v>33</v>
-      </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -1650,66 +1596,44 @@
       <c r="H2" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>1</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="1">
-        <f>Operations!D19</f>
-        <v>16</v>
-      </c>
+      <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="P3" s="1">
-        <v>16</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
-      </c>
-      <c r="P4" s="1">
-        <v>16</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
-      </c>
-      <c r="P5" s="1">
-        <v>16</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <f>C6+D6*P2</f>
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
@@ -1718,2080 +1642,1442 @@
         <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I6" s="5">
+        <v>79</v>
+      </c>
+      <c r="I6" s="4">
         <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" s="1">
-        <v>16</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E7">
         <f>C7+D7*P2</f>
         <v>0</v>
       </c>
-      <c r="P7" s="1">
-        <v>16</v>
-      </c>
+      <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E8">
         <f>C8+D8*P2</f>
         <v>0</v>
       </c>
-      <c r="P8" s="1">
-        <v>16</v>
-      </c>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E9">
         <f>C9+D9*P2</f>
         <v>0</v>
       </c>
-      <c r="P9" s="1">
-        <v>16</v>
-      </c>
+      <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <f>C10+D10*P5</f>
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G10" t="s">
         <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="5">
+        <v>86</v>
+      </c>
+      <c r="I10" s="4">
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="P10" s="1">
-        <v>16</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s">
-        <v>217</v>
-      </c>
-      <c r="P11" s="1">
-        <v>16</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f>C12+D12*P2</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="G12" t="s">
         <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I12" s="5">
+        <v>91</v>
+      </c>
+      <c r="I12" s="4">
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P12" s="1">
-        <v>16</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>229</v>
-      </c>
-      <c r="P13" s="1">
-        <v>16</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f>C14+D14*P8</f>
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H14" t="s">
-        <v>100</v>
-      </c>
-      <c r="I14" s="5">
+        <v>95</v>
+      </c>
+      <c r="I14" s="4">
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P14" s="1">
-        <v>16</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B15" t="s">
-        <v>232</v>
-      </c>
-      <c r="P15" s="1">
-        <v>16</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <f>C16+D16*P8</f>
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H16" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" s="5">
+        <v>99</v>
+      </c>
+      <c r="I16" s="4">
         <v>1</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P16" s="1">
-        <v>16</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
-      </c>
-      <c r="P17" s="1">
-        <v>16</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="10">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f>C18+D18*P5</f>
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="G18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="5">
+        <v>105</v>
+      </c>
+      <c r="I18" s="4">
         <v>1</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P18" s="1">
-        <v>16</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s">
-        <v>233</v>
-      </c>
-      <c r="P19" s="1">
-        <v>16</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" s="10">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <f>C20+D20*P11</f>
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H20" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" s="5">
+        <v>110</v>
+      </c>
+      <c r="I20" s="4">
         <v>1</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="P20" s="1">
-        <v>16</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B21" t="s">
-        <v>235</v>
-      </c>
-      <c r="P21" s="1">
-        <v>16</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
-        <v>234</v>
-      </c>
-      <c r="P22" s="1">
-        <v>16</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="10">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <f>C23+D23*P11</f>
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="G23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" s="5">
+        <v>114</v>
+      </c>
+      <c r="I23" s="4">
         <v>1</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="P23" s="1">
-        <v>16</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>281</v>
-      </c>
-      <c r="P24" s="1">
-        <v>16</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="P24" s="1"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
-      </c>
-      <c r="P25" s="1">
-        <v>16</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B26" t="s">
-        <v>220</v>
-      </c>
-      <c r="P26" s="1">
-        <v>16</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="P26" s="1"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B27" t="s">
-        <v>236</v>
-      </c>
-      <c r="P27" s="1">
-        <v>16</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="P27" s="1"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
-      </c>
-      <c r="P28" s="1">
-        <v>16</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="P28" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" s="10">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <f>C29+D29*P8</f>
-        <v>17</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H29" t="s">
-        <v>122</v>
-      </c>
-      <c r="I29" s="5">
+        <v>117</v>
+      </c>
+      <c r="I29" s="4">
         <v>1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="P29" s="1">
-        <v>16</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="P29" s="1"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B30" t="s">
-        <v>279</v>
-      </c>
-      <c r="P30" s="1">
-        <v>16</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="P30" s="1"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B31" t="s">
-        <v>280</v>
-      </c>
-      <c r="P31" s="1">
-        <v>16</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="P31" s="1"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="10">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <f>C32+D32*P14</f>
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="G32" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H32" t="s">
-        <v>125</v>
-      </c>
-      <c r="I32" s="5">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="P32" s="1">
-        <v>16</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="I32" s="9">
+        <v>1</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33">
-        <v>5</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" s="10">
-        <v>4</v>
-      </c>
-      <c r="E33">
-        <f>C33+D33*P14</f>
-        <v>65</v>
-      </c>
-      <c r="G33" t="s">
-        <v>129</v>
-      </c>
-      <c r="H33" t="s">
-        <v>128</v>
-      </c>
-      <c r="I33" s="5">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="P33" s="1">
-        <v>16</v>
+        <v>224</v>
+      </c>
+      <c r="B33" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>230</v>
-      </c>
-      <c r="B34" t="s">
-        <v>221</v>
-      </c>
-      <c r="P34" s="1">
-        <v>16</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B35" t="s">
-        <v>222</v>
-      </c>
-      <c r="P35" s="1">
-        <v>16</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B36" t="s">
-        <v>223</v>
-      </c>
-      <c r="C36" t="s">
-        <v>224</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="E36" t="s">
-        <v>226</v>
-      </c>
-      <c r="P36" s="1">
-        <v>16</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="P36" s="1"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B37" t="s">
-        <v>227</v>
-      </c>
-      <c r="P37" s="1">
-        <v>16</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="C37" t="s">
+        <v>217</v>
+      </c>
+      <c r="D37" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" t="s">
+        <v>219</v>
+      </c>
+      <c r="P37" s="1"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
-      </c>
-      <c r="P38" s="1">
-        <v>16</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="P38" s="1"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" s="10">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <f>C39+D39*P11</f>
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>114</v>
-      </c>
-      <c r="H39" t="s">
-        <v>132</v>
-      </c>
-      <c r="I39" s="5">
-        <v>1</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="P39" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B39" t="s">
+        <v>231</v>
+      </c>
+      <c r="P39" s="1"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>231</v>
-      </c>
-      <c r="B40" t="s">
-        <v>239</v>
-      </c>
-      <c r="P40" s="1">
-        <v>16</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G40" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" t="s">
+        <v>127</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="P40" s="1"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" s="10">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <f>C41+D41*P17</f>
-        <v>17</v>
-      </c>
-      <c r="G41" t="s">
-        <v>137</v>
-      </c>
-      <c r="H41" t="s">
-        <v>136</v>
-      </c>
-      <c r="I41" s="5">
-        <v>1</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="P41" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B41" t="s">
+        <v>232</v>
+      </c>
+      <c r="P41" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>231</v>
-      </c>
-      <c r="B42" t="s">
-        <v>240</v>
-      </c>
-      <c r="P42" s="1">
-        <v>16</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="G42" t="s">
+        <v>132</v>
+      </c>
+      <c r="H42" t="s">
+        <v>131</v>
+      </c>
+      <c r="I42" s="4">
+        <v>1</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P42" s="1"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B43" t="s">
-        <v>241</v>
-      </c>
-      <c r="P43" s="1">
-        <v>16</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="P43" s="1"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44" s="10">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <f>C44+D44*P17</f>
-        <v>16</v>
-      </c>
-      <c r="G44" t="s">
-        <v>101</v>
-      </c>
-      <c r="H44" t="s">
-        <v>139</v>
-      </c>
-      <c r="I44" s="5">
-        <v>1</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="P44" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B44" t="s">
+        <v>234</v>
+      </c>
+      <c r="P44" s="1"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>230</v>
-      </c>
-      <c r="B45" t="s">
-        <v>242</v>
-      </c>
-      <c r="P45" s="1">
-        <v>16</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G45" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" t="s">
+        <v>134</v>
+      </c>
+      <c r="I45" s="4">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="P45" s="1"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>141</v>
-      </c>
-      <c r="B46">
-        <v>2</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" s="10">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <f>C46+D46*P14</f>
-        <v>2</v>
-      </c>
-      <c r="G46" t="s">
-        <v>129</v>
-      </c>
-      <c r="H46" t="s">
-        <v>143</v>
-      </c>
-      <c r="I46" s="5">
-        <v>1</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P46" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B46" t="s">
+        <v>235</v>
+      </c>
+      <c r="P46" s="1"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>231</v>
-      </c>
-      <c r="B47" t="s">
-        <v>243</v>
-      </c>
-      <c r="P47" s="1">
-        <v>16</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="G47" t="s">
+        <v>124</v>
+      </c>
+      <c r="H47" t="s">
+        <v>138</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P47" s="1"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B48" t="s">
-        <v>244</v>
-      </c>
-      <c r="P48" s="1">
-        <v>16</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="P48" s="1"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49">
-        <v>2</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49" s="10">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <f>C49+D49*P20</f>
-        <v>2</v>
-      </c>
-      <c r="G49" t="s">
-        <v>129</v>
-      </c>
-      <c r="H49" t="s">
-        <v>145</v>
-      </c>
-      <c r="I49" s="5">
-        <v>1</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="P49" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B49" t="s">
+        <v>237</v>
+      </c>
+      <c r="P49" s="1"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>231</v>
-      </c>
-      <c r="B50" t="s">
-        <v>243</v>
-      </c>
-      <c r="P50" s="1">
-        <v>16</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="G50" t="s">
+        <v>124</v>
+      </c>
+      <c r="H50" t="s">
+        <v>140</v>
+      </c>
+      <c r="I50" s="4">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="P50" s="1"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B51" t="s">
-        <v>244</v>
-      </c>
-      <c r="P51" s="1">
-        <v>16</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="P51" s="1"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>148</v>
-      </c>
-      <c r="B52">
-        <v>2</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52" s="10">
-        <v>2</v>
-      </c>
-      <c r="E52">
-        <f>C52+D52*P20</f>
-        <v>32</v>
-      </c>
-      <c r="G52" t="s">
-        <v>150</v>
-      </c>
-      <c r="H52" t="s">
-        <v>149</v>
-      </c>
-      <c r="I52" s="5">
-        <v>1</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="P52" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B52" t="s">
+        <v>237</v>
+      </c>
+      <c r="P52" s="1"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>230</v>
-      </c>
-      <c r="B53" t="s">
-        <v>245</v>
-      </c>
-      <c r="P53" s="1">
-        <v>16</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="G53" t="s">
+        <v>145</v>
+      </c>
+      <c r="H53" t="s">
+        <v>144</v>
+      </c>
+      <c r="I53" s="4">
+        <v>1</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="P53" s="1"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B54" t="s">
-        <v>246</v>
-      </c>
-      <c r="P54" s="1">
-        <v>16</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="P54" s="1"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>153</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55" s="10">
-        <v>2</v>
-      </c>
-      <c r="E55">
-        <f>C55+D55*P17</f>
-        <v>32</v>
-      </c>
-      <c r="G55" t="s">
-        <v>154</v>
-      </c>
-      <c r="H55" t="s">
-        <v>152</v>
-      </c>
-      <c r="I55" s="5">
-        <v>1</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="P55" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B55" t="s">
+        <v>239</v>
+      </c>
+      <c r="P55" s="1"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>230</v>
-      </c>
-      <c r="B56" t="s">
-        <v>247</v>
-      </c>
-      <c r="P56" s="1">
-        <v>16</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="G56" t="s">
+        <v>149</v>
+      </c>
+      <c r="H56" t="s">
+        <v>147</v>
+      </c>
+      <c r="I56" s="4">
+        <v>1</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="P56" s="1"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>155</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57" s="10">
-        <v>2</v>
-      </c>
-      <c r="E57">
-        <f>C57+D57*P18</f>
-        <v>32</v>
-      </c>
-      <c r="G57" t="s">
-        <v>154</v>
-      </c>
-      <c r="H57" t="s">
-        <v>152</v>
-      </c>
-      <c r="I57" s="5">
-        <v>1</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="P57" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B57" t="s">
+        <v>240</v>
+      </c>
+      <c r="P57" s="1"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>230</v>
-      </c>
-      <c r="B58" t="s">
-        <v>248</v>
-      </c>
-      <c r="P58" s="1">
-        <v>16</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="G58" t="s">
+        <v>149</v>
+      </c>
+      <c r="H58" t="s">
+        <v>147</v>
+      </c>
+      <c r="I58" s="4">
+        <v>1</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P58" s="1"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>157</v>
-      </c>
-      <c r="B59">
-        <v>2</v>
-      </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59" s="10">
-        <v>2</v>
-      </c>
-      <c r="E59">
-        <f>C59+D59*P19</f>
-        <v>32</v>
-      </c>
-      <c r="G59" t="s">
-        <v>160</v>
-      </c>
-      <c r="H59" t="s">
-        <v>159</v>
-      </c>
-      <c r="I59" s="5">
-        <v>1</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="P59" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B59" t="s">
+        <v>241</v>
+      </c>
+      <c r="P59" s="1"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>230</v>
-      </c>
-      <c r="B60" t="s">
-        <v>250</v>
-      </c>
-      <c r="P60" s="1">
-        <v>16</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="G60" t="s">
+        <v>155</v>
+      </c>
+      <c r="H60" t="s">
+        <v>154</v>
+      </c>
+      <c r="I60" s="4">
+        <v>1</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="P60" s="1"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B61" t="s">
-        <v>249</v>
-      </c>
-      <c r="P61" s="1">
-        <v>16</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="P61" s="1"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>161</v>
-      </c>
-      <c r="B62">
-        <v>4</v>
-      </c>
-      <c r="C62">
-        <v>4</v>
-      </c>
-      <c r="D62" s="10">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <f>C62+D62*P20</f>
-        <v>4</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G62" t="s">
-        <v>150</v>
-      </c>
-      <c r="H62" t="s">
-        <v>163</v>
-      </c>
-      <c r="I62" s="5">
-        <v>1</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="P62" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B62" t="s">
+        <v>242</v>
+      </c>
+      <c r="P62" s="1"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>231</v>
-      </c>
-      <c r="B63" t="s">
-        <v>251</v>
-      </c>
-      <c r="P63" s="1">
-        <v>16</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63" t="s">
+        <v>145</v>
+      </c>
+      <c r="H63" t="s">
+        <v>158</v>
+      </c>
+      <c r="I63" s="4">
+        <v>1</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P63" s="1"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B64" t="s">
-        <v>252</v>
-      </c>
-      <c r="P64" s="1">
-        <v>16</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="P64" s="1"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B65" t="s">
-        <v>253</v>
-      </c>
-      <c r="P65" s="1">
-        <v>16</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="P65" s="1"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B66" t="s">
-        <v>254</v>
-      </c>
-      <c r="P66" s="1">
-        <v>16</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="P66" s="1"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67" s="10">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <f>C67+D67*P21</f>
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>56</v>
-      </c>
-      <c r="G67" t="s">
-        <v>150</v>
-      </c>
-      <c r="H67" t="s">
-        <v>163</v>
-      </c>
-      <c r="I67" s="5">
-        <v>1</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P67" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B67" t="s">
+        <v>247</v>
+      </c>
+      <c r="P67" s="1"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>231</v>
-      </c>
-      <c r="B68" t="s">
-        <v>255</v>
-      </c>
-      <c r="P68" s="1">
-        <v>16</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="F68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68" t="s">
+        <v>145</v>
+      </c>
+      <c r="H68" t="s">
+        <v>158</v>
+      </c>
+      <c r="I68" s="4">
+        <v>1</v>
+      </c>
+      <c r="J68" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="P68" s="1"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>165</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69" s="10">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <f>C69+D69*P22</f>
-        <v>1</v>
-      </c>
-      <c r="F69" t="s">
-        <v>56</v>
-      </c>
-      <c r="G69" t="s">
-        <v>150</v>
-      </c>
-      <c r="H69" t="s">
-        <v>163</v>
-      </c>
-      <c r="I69" s="5">
-        <v>1</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="P69" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B69" t="s">
+        <v>248</v>
+      </c>
+      <c r="P69" s="1"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>231</v>
-      </c>
-      <c r="B70" t="s">
-        <v>256</v>
-      </c>
-      <c r="P70" s="1">
-        <v>16</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="F70" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" t="s">
+        <v>145</v>
+      </c>
+      <c r="H70" t="s">
+        <v>158</v>
+      </c>
+      <c r="I70" s="4">
+        <v>1</v>
+      </c>
+      <c r="J70" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P70" s="1"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>166</v>
-      </c>
-      <c r="B71">
-        <v>6</v>
-      </c>
-      <c r="C71">
-        <v>6</v>
-      </c>
-      <c r="D71" s="10">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <f>C71+D71*P23</f>
-        <v>6</v>
-      </c>
-      <c r="F71" t="s">
-        <v>56</v>
-      </c>
-      <c r="G71" t="s">
-        <v>150</v>
-      </c>
-      <c r="H71" t="s">
-        <v>163</v>
-      </c>
-      <c r="I71" s="5">
-        <v>1</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="P71" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B71" t="s">
+        <v>249</v>
+      </c>
+      <c r="P71" s="1"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>231</v>
-      </c>
-      <c r="B72" t="s">
-        <v>257</v>
-      </c>
-      <c r="P72" s="1">
-        <v>16</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="F72" t="s">
+        <v>56</v>
+      </c>
+      <c r="G72" t="s">
+        <v>145</v>
+      </c>
+      <c r="H72" t="s">
+        <v>158</v>
+      </c>
+      <c r="I72" s="4">
+        <v>1</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="P72" s="1"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B73" t="s">
-        <v>258</v>
-      </c>
-      <c r="P73" s="1">
-        <v>16</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="P73" s="1"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B74" t="s">
-        <v>259</v>
-      </c>
-      <c r="P74" s="1">
-        <v>16</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="P74" s="1"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B75" t="s">
-        <v>260</v>
-      </c>
-      <c r="P75" s="1">
-        <v>16</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="P75" s="1"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B76" t="s">
-        <v>261</v>
-      </c>
-      <c r="P76" s="1">
-        <v>16</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="P76" s="1"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B77" t="s">
-        <v>262</v>
-      </c>
-      <c r="P77" s="1">
-        <v>16</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="P77" s="1"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78" s="10">
-        <v>1</v>
-      </c>
-      <c r="E78">
-        <f>C78+D78*P24</f>
-        <v>16</v>
-      </c>
-      <c r="G78" t="s">
-        <v>160</v>
-      </c>
-      <c r="H78" t="s">
-        <v>171</v>
-      </c>
-      <c r="I78" s="5">
-        <v>1</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="P78" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B78" t="s">
+        <v>255</v>
+      </c>
+      <c r="P78" s="1"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>230</v>
-      </c>
-      <c r="B79" t="s">
-        <v>263</v>
-      </c>
-      <c r="C79" t="s">
-        <v>264</v>
-      </c>
-      <c r="P79" s="1">
-        <v>16</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="G79" t="s">
+        <v>155</v>
+      </c>
+      <c r="H79" t="s">
+        <v>166</v>
+      </c>
+      <c r="I79" s="4">
+        <v>1</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P79" s="1"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>173</v>
-      </c>
-      <c r="B80">
-        <v>6</v>
-      </c>
-      <c r="C80">
-        <v>3</v>
-      </c>
-      <c r="D80" s="10">
-        <v>3</v>
-      </c>
-      <c r="E80">
-        <f>C80+D80*P25</f>
-        <v>51</v>
-      </c>
-      <c r="F80" t="s">
-        <v>176</v>
-      </c>
-      <c r="G80" t="s">
-        <v>154</v>
-      </c>
-      <c r="H80" t="s">
-        <v>175</v>
-      </c>
-      <c r="I80" s="5">
-        <v>1</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="P80" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B80" t="s">
+        <v>256</v>
+      </c>
+      <c r="C80" t="s">
+        <v>257</v>
+      </c>
+      <c r="P80" s="1"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>230</v>
-      </c>
-      <c r="B81" t="s">
-        <v>265</v>
-      </c>
-      <c r="P81" s="1">
-        <v>16</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="F81" t="s">
+        <v>171</v>
+      </c>
+      <c r="G81" t="s">
+        <v>149</v>
+      </c>
+      <c r="H81" t="s">
+        <v>170</v>
+      </c>
+      <c r="I81" s="4">
+        <v>1</v>
+      </c>
+      <c r="J81" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="P81" s="1"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s">
-        <v>266</v>
-      </c>
-      <c r="P82" s="1">
-        <v>16</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="P82" s="1"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B83" t="s">
-        <v>267</v>
-      </c>
-      <c r="P83" s="1">
-        <v>16</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="P83" s="1"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B84" t="s">
-        <v>268</v>
-      </c>
-      <c r="P84" s="1">
-        <v>16</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="P84" s="1"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B85" t="s">
-        <v>269</v>
-      </c>
-      <c r="P85" s="1">
-        <v>16</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="P85" s="1"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B86" t="s">
-        <v>270</v>
-      </c>
-      <c r="P86" s="1">
-        <v>16</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="P86" s="1"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>177</v>
-      </c>
-      <c r="B87">
-        <v>2</v>
-      </c>
-      <c r="C87">
-        <v>0</v>
-      </c>
-      <c r="D87" s="10">
-        <v>2</v>
-      </c>
-      <c r="E87">
-        <f>C87+D87*P26</f>
-        <v>32</v>
-      </c>
-      <c r="G87" t="s">
-        <v>154</v>
-      </c>
-      <c r="H87" t="s">
-        <v>179</v>
-      </c>
-      <c r="I87" s="5">
-        <v>1</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="P87" s="1">
-        <v>16</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B87" t="s">
+        <v>263</v>
+      </c>
+      <c r="P87" s="1"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>230</v>
-      </c>
-      <c r="B88" t="s">
-        <v>271</v>
-      </c>
-      <c r="P88" s="1">
-        <v>16</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="G88" t="s">
+        <v>149</v>
+      </c>
+      <c r="H88" t="s">
+        <v>174</v>
+      </c>
+      <c r="I88" s="4">
+        <v>1</v>
+      </c>
+      <c r="J88" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P88" s="1"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B89" t="s">
-        <v>272</v>
-      </c>
-      <c r="P89" s="1">
-        <v>16</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="P89" s="1"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>180</v>
-      </c>
-      <c r="B90">
-        <v>2</v>
-      </c>
-      <c r="C90">
-        <v>1</v>
-      </c>
-      <c r="D90" s="10">
-        <v>1</v>
-      </c>
-      <c r="E90">
-        <f>C90+D90*P27</f>
-        <v>17</v>
-      </c>
-      <c r="G90" t="s">
-        <v>154</v>
-      </c>
-      <c r="H90" t="s">
-        <v>182</v>
-      </c>
-      <c r="I90" s="5">
-        <v>1</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="P90" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B90" t="s">
+        <v>265</v>
+      </c>
+      <c r="P90" s="1"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>231</v>
-      </c>
-      <c r="B91" t="s">
-        <v>273</v>
-      </c>
-      <c r="P91" s="1">
-        <v>16</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G91" t="s">
+        <v>149</v>
+      </c>
+      <c r="H91" t="s">
+        <v>177</v>
+      </c>
+      <c r="I91" s="4">
+        <v>1</v>
+      </c>
+      <c r="J91" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="P91" s="1"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B92" t="s">
-        <v>274</v>
-      </c>
-      <c r="P92" s="1">
-        <v>16</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="P92" s="1"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
-      </c>
-      <c r="B93">
-        <v>1</v>
-      </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-      <c r="D93" s="10">
-        <v>1</v>
-      </c>
-      <c r="E93">
-        <f>C93+D93*P28</f>
-        <v>16</v>
-      </c>
-      <c r="G93" t="s">
-        <v>154</v>
-      </c>
-      <c r="H93" t="s">
-        <v>185</v>
-      </c>
-      <c r="I93" s="5">
-        <v>1</v>
-      </c>
-      <c r="J93" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="P93" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B93" t="s">
+        <v>267</v>
+      </c>
+      <c r="P93" s="1"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>230</v>
-      </c>
-      <c r="B94" t="s">
-        <v>275</v>
-      </c>
-      <c r="P94" s="1">
-        <v>16</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="G94" t="s">
+        <v>149</v>
+      </c>
+      <c r="H94" t="s">
+        <v>180</v>
+      </c>
+      <c r="I94" s="4">
+        <v>1</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="P94" s="1"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>187</v>
-      </c>
-      <c r="B95">
-        <v>3</v>
-      </c>
-      <c r="C95">
-        <v>3</v>
-      </c>
-      <c r="D95" s="10">
-        <v>0</v>
-      </c>
-      <c r="E95">
-        <f>C95+D95*P29</f>
-        <v>3</v>
-      </c>
-      <c r="F95" t="s">
-        <v>188</v>
-      </c>
-      <c r="G95" t="s">
-        <v>101</v>
-      </c>
-      <c r="H95" t="s">
-        <v>189</v>
-      </c>
-      <c r="I95" s="5">
-        <v>1</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="P95" s="1">
-        <v>16</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B95" t="s">
+        <v>268</v>
+      </c>
+      <c r="P95" s="1"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>231</v>
-      </c>
-      <c r="B96" t="s">
-        <v>276</v>
-      </c>
-      <c r="P96" s="1">
-        <v>16</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="F96" t="s">
+        <v>183</v>
+      </c>
+      <c r="G96" t="s">
+        <v>96</v>
+      </c>
+      <c r="H96" t="s">
+        <v>184</v>
+      </c>
+      <c r="I96" s="4">
+        <v>1</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="P96" s="1"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B97" t="s">
-        <v>277</v>
-      </c>
-      <c r="P97" s="1">
-        <v>16</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="P97" s="1"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B98" t="s">
-        <v>278</v>
-      </c>
-      <c r="P98" s="1">
-        <v>16</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="P98" s="1"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B99">
-        <v>0</v>
-      </c>
-      <c r="C99">
-        <v>0</v>
-      </c>
-      <c r="D99" s="10">
-        <v>3</v>
-      </c>
-      <c r="E99">
-        <f>C99+D99*P30</f>
-        <v>48</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="A99" t="s">
+        <v>224</v>
+      </c>
+      <c r="B99" t="s">
+        <v>271</v>
+      </c>
+      <c r="P99" s="1"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F100" t="s">
+        <v>185</v>
+      </c>
+      <c r="G100" t="s">
+        <v>109</v>
+      </c>
+      <c r="H100" t="s">
+        <v>187</v>
+      </c>
+      <c r="I100" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="P100" s="1"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
         <v>190</v>
       </c>
-      <c r="G99" t="s">
-        <v>114</v>
-      </c>
-      <c r="H99" t="s">
-        <v>192</v>
-      </c>
-      <c r="I99" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="J99" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="P99" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F100" t="s">
-        <v>195</v>
-      </c>
-      <c r="I100" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P100" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E101">
-        <f t="shared" ref="E101:E109" si="0">C101+D101*P32</f>
-        <v>0</v>
-      </c>
-      <c r="F101" t="s">
-        <v>196</v>
-      </c>
-      <c r="I101" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P101" s="1">
-        <v>16</v>
-      </c>
+      <c r="I101" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P101" s="1"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E102">
-        <f t="shared" si="0"/>
+        <f>C102+D102*P32</f>
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>197</v>
-      </c>
-      <c r="I102" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P102" s="1">
-        <v>16</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P102" s="1"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>198</v>
-      </c>
       <c r="E103">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E103:E110" si="0">C103+D103*P34</f>
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>199</v>
-      </c>
-      <c r="I103" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="P103" s="1">
-        <v>16</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P103" s="1"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>201</v>
-      </c>
-      <c r="B104" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I104" s="6" t="s">
+      <c r="F104" t="s">
         <v>194</v>
       </c>
-      <c r="P104" s="1">
-        <v>16</v>
-      </c>
+      <c r="I104" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="P104" s="1"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>203</v>
-      </c>
-      <c r="B105">
-        <v>0</v>
-      </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105" s="10">
-        <v>1</v>
+        <v>196</v>
+      </c>
+      <c r="B105" t="s">
+        <v>189</v>
       </c>
       <c r="E105">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="F105" t="s">
-        <v>202</v>
-      </c>
-      <c r="I105" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P105" s="1">
-        <v>16</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I105" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P105" s="1"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B106">
         <v>0</v>
       </c>
       <c r="C106">
-        <v>1</v>
-      </c>
-      <c r="D106" s="10">
+        <v>0</v>
+      </c>
+      <c r="D106">
         <v>1</v>
       </c>
       <c r="E106">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>206</v>
-      </c>
-      <c r="I106" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="J106" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="P106" s="1">
-        <v>16</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P106" s="1"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>200</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
       <c r="E107">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>207</v>
-      </c>
-      <c r="I107" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P107" s="1">
-        <v>16</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="I107" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="P107" s="1"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>208</v>
-      </c>
-      <c r="B108" t="s">
-        <v>209</v>
-      </c>
-      <c r="C108">
-        <v>1</v>
-      </c>
-      <c r="D108" s="10">
-        <v>0</v>
-      </c>
       <c r="E108">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>210</v>
-      </c>
-      <c r="I108" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="P108" s="1">
-        <v>16</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P108" s="1"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
       <c r="E109">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F109" t="s">
+        <v>204</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="P109" s="1"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F109" t="s">
-        <v>212</v>
-      </c>
-      <c r="I109" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P109" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F110" t="s">
-        <v>214</v>
-      </c>
-      <c r="I110" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P110" s="1">
-        <v>16</v>
-      </c>
+      <c r="I110" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P110" s="1"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
-        <v>215</v>
-      </c>
-      <c r="I111" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P111" s="1">
-        <v>16</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="I111" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P111" s="1"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F112" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I112" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="P112" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="113" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P113" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="114" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P114" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="115" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P115" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="116" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P116" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="117" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P117" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="118" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P118" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="119" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P119" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="120" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P120" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="121" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P121" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="122" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P122" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="123" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P123" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="124" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P124" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="125" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P125" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="126" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P126" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="127" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P127" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="128" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P128" s="1">
-        <v>16</v>
-      </c>
+      <c r="F112" t="s">
+        <v>208</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P112" s="1"/>
+    </row>
+    <row r="113" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F113" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="P113" s="1"/>
+    </row>
+    <row r="114" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P114" s="1"/>
+    </row>
+    <row r="115" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P115" s="1"/>
+    </row>
+    <row r="116" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P116" s="1"/>
+    </row>
+    <row r="117" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P117" s="1"/>
+    </row>
+    <row r="118" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P118" s="1"/>
+    </row>
+    <row r="119" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P119" s="1"/>
+    </row>
+    <row r="120" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P120" s="1"/>
+    </row>
+    <row r="121" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P121" s="1"/>
+    </row>
+    <row r="122" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P122" s="1"/>
+    </row>
+    <row r="123" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P123" s="1"/>
+    </row>
+    <row r="124" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P124" s="1"/>
+    </row>
+    <row r="125" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P125" s="1"/>
+    </row>
+    <row r="126" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P126" s="1"/>
+    </row>
+    <row r="127" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P127" s="1"/>
+    </row>
+    <row r="128" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="P128" s="1"/>
     </row>
     <row r="129" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P129" s="1">
-        <v>16</v>
-      </c>
+      <c r="P129" s="1"/>
     </row>
     <row r="130" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P130" s="1">
-        <v>16</v>
-      </c>
+      <c r="P130" s="1"/>
+    </row>
+    <row r="131" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P131" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3807,31 +3093,31 @@
     <hyperlink ref="J23" r:id="rId9" xr:uid="{F85FDA03-2340-4E6F-BDA0-4D7B510CD82B}"/>
     <hyperlink ref="J29" r:id="rId10" xr:uid="{E7631147-1D00-497E-ADD3-2B2DB3DC3B32}"/>
     <hyperlink ref="J32" r:id="rId11" xr:uid="{D71B4294-1913-47E3-AF74-4EC78E726A1C}"/>
-    <hyperlink ref="J33" r:id="rId12" xr:uid="{F93255C8-DF3F-43BA-AD4C-A8E80732B132}"/>
-    <hyperlink ref="J39" r:id="rId13" xr:uid="{CAED3824-A4C7-4CCF-B3BD-36731286A453}"/>
-    <hyperlink ref="J41" r:id="rId14" xr:uid="{72733251-81F4-429A-BC69-7E42806BAAB4}"/>
-    <hyperlink ref="J44" r:id="rId15" xr:uid="{776D380D-752E-4EFB-9866-FC18DE6ECC82}"/>
-    <hyperlink ref="J46" r:id="rId16" xr:uid="{70ACD712-33B8-4D08-81E7-2E40C82C1029}"/>
-    <hyperlink ref="J49" r:id="rId17" xr:uid="{2C55EC1D-70BC-415E-9A54-6B6889679D43}"/>
-    <hyperlink ref="J52" r:id="rId18" xr:uid="{9D95D7E8-ACAA-46C0-92C5-81C743CACE8A}"/>
-    <hyperlink ref="J55" r:id="rId19" xr:uid="{DBD5001E-FD5C-49ED-8D2E-E2F1BF6C8CC1}"/>
-    <hyperlink ref="J57" r:id="rId20" xr:uid="{67AD61E2-1C52-4087-BAB4-B64448CC9F4D}"/>
-    <hyperlink ref="J59" r:id="rId21" xr:uid="{5D7188A2-C9F7-41CE-82D4-3B2A3D5EE3F7}"/>
-    <hyperlink ref="J62" r:id="rId22" xr:uid="{638C9C06-C9E4-4CC8-B93A-A360377F7713}"/>
-    <hyperlink ref="J67" r:id="rId23" xr:uid="{BC529E61-7341-48DF-8AC1-BB21A6063CD3}"/>
-    <hyperlink ref="J69" r:id="rId24" xr:uid="{E75414B1-CEB6-4293-9B2E-42028D229848}"/>
-    <hyperlink ref="J71" r:id="rId25" xr:uid="{BC9143FB-8381-4C68-9B5F-CF7DB1497F63}"/>
-    <hyperlink ref="J78" r:id="rId26" xr:uid="{1DBCAFCF-5131-47AE-9C12-8E42CD256740}"/>
-    <hyperlink ref="J80" r:id="rId27" xr:uid="{08700766-0E5A-4C62-BFAB-F95492D1F1CB}"/>
-    <hyperlink ref="J87" r:id="rId28" xr:uid="{B8E82F50-D15B-4556-9088-2F9C4D09091E}"/>
-    <hyperlink ref="J90" r:id="rId29" xr:uid="{D5E29CDB-ED2B-4A96-AE32-8141A2955370}"/>
-    <hyperlink ref="J93" r:id="rId30" xr:uid="{8F4B9E06-3CED-47F1-B93F-1207A48E16B5}"/>
-    <hyperlink ref="J95" r:id="rId31" xr:uid="{98E8F283-8F69-4CC5-A4FF-CB5301CF9F96}"/>
-    <hyperlink ref="J103" r:id="rId32" xr:uid="{439D2314-9B22-415F-A5A1-3563D4642932}"/>
-    <hyperlink ref="J99" r:id="rId33" xr:uid="{8C102FE7-D93B-4BD9-A57B-C72DAD4EDBA2}"/>
-    <hyperlink ref="J106" r:id="rId34" xr:uid="{E62C70A8-FDB5-421A-AFA1-E3262C592104}"/>
-    <hyperlink ref="J108" r:id="rId35" xr:uid="{C2297CF9-E7ED-417B-968E-0AAE230EDB1A}"/>
-    <hyperlink ref="F112" r:id="rId36" xr:uid="{5E6A4597-E97E-48FB-96BA-F6F33955E589}"/>
+    <hyperlink ref="J34" r:id="rId12" xr:uid="{F93255C8-DF3F-43BA-AD4C-A8E80732B132}"/>
+    <hyperlink ref="J40" r:id="rId13" xr:uid="{CAED3824-A4C7-4CCF-B3BD-36731286A453}"/>
+    <hyperlink ref="J42" r:id="rId14" xr:uid="{72733251-81F4-429A-BC69-7E42806BAAB4}"/>
+    <hyperlink ref="J45" r:id="rId15" xr:uid="{776D380D-752E-4EFB-9866-FC18DE6ECC82}"/>
+    <hyperlink ref="J47" r:id="rId16" xr:uid="{70ACD712-33B8-4D08-81E7-2E40C82C1029}"/>
+    <hyperlink ref="J50" r:id="rId17" xr:uid="{2C55EC1D-70BC-415E-9A54-6B6889679D43}"/>
+    <hyperlink ref="J53" r:id="rId18" xr:uid="{9D95D7E8-ACAA-46C0-92C5-81C743CACE8A}"/>
+    <hyperlink ref="J56" r:id="rId19" xr:uid="{DBD5001E-FD5C-49ED-8D2E-E2F1BF6C8CC1}"/>
+    <hyperlink ref="J58" r:id="rId20" xr:uid="{67AD61E2-1C52-4087-BAB4-B64448CC9F4D}"/>
+    <hyperlink ref="J60" r:id="rId21" xr:uid="{5D7188A2-C9F7-41CE-82D4-3B2A3D5EE3F7}"/>
+    <hyperlink ref="J63" r:id="rId22" xr:uid="{638C9C06-C9E4-4CC8-B93A-A360377F7713}"/>
+    <hyperlink ref="J68" r:id="rId23" xr:uid="{BC529E61-7341-48DF-8AC1-BB21A6063CD3}"/>
+    <hyperlink ref="J70" r:id="rId24" xr:uid="{E75414B1-CEB6-4293-9B2E-42028D229848}"/>
+    <hyperlink ref="J72" r:id="rId25" xr:uid="{BC9143FB-8381-4C68-9B5F-CF7DB1497F63}"/>
+    <hyperlink ref="J79" r:id="rId26" xr:uid="{1DBCAFCF-5131-47AE-9C12-8E42CD256740}"/>
+    <hyperlink ref="J81" r:id="rId27" xr:uid="{08700766-0E5A-4C62-BFAB-F95492D1F1CB}"/>
+    <hyperlink ref="J88" r:id="rId28" xr:uid="{B8E82F50-D15B-4556-9088-2F9C4D09091E}"/>
+    <hyperlink ref="J91" r:id="rId29" xr:uid="{D5E29CDB-ED2B-4A96-AE32-8141A2955370}"/>
+    <hyperlink ref="J94" r:id="rId30" xr:uid="{8F4B9E06-3CED-47F1-B93F-1207A48E16B5}"/>
+    <hyperlink ref="J96" r:id="rId31" xr:uid="{98E8F283-8F69-4CC5-A4FF-CB5301CF9F96}"/>
+    <hyperlink ref="J104" r:id="rId32" xr:uid="{439D2314-9B22-415F-A5A1-3563D4642932}"/>
+    <hyperlink ref="J100" r:id="rId33" xr:uid="{8C102FE7-D93B-4BD9-A57B-C72DAD4EDBA2}"/>
+    <hyperlink ref="J107" r:id="rId34" xr:uid="{E62C70A8-FDB5-421A-AFA1-E3262C592104}"/>
+    <hyperlink ref="J109" r:id="rId35" xr:uid="{C2297CF9-E7ED-417B-968E-0AAE230EDB1A}"/>
+    <hyperlink ref="F113" r:id="rId36" xr:uid="{5E6A4597-E97E-48FB-96BA-F6F33955E589}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4012,7 +3298,7 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4189,39 +3475,39 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="8">
+      <c r="B24" s="7">
         <v>13</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="8">
+      <c r="B25" s="7">
         <v>14</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D26" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4256,7 +3542,7 @@
         <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="F30" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
updated script to show more details, run again to get more statistics
</commit_message>
<xml_diff>
--- a/MiTRE/MitreOperations.xlsx
+++ b/MiTRE/MitreOperations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AssistantsTesterGithub\MiTRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C16F04-AACE-48DA-9CF7-BC5F199F3A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63F12B1-2219-49D1-9EF1-CA44A9A04C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="OperatiiExistente" sheetId="2" r:id="rId1"/>
+    <sheet name="ImplementedOperations" sheetId="2" r:id="rId1"/>
     <sheet name="Operations" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -498,9 +498,6 @@
     <t>Credential Access</t>
   </si>
   <si>
-    <t>Variants</t>
-  </si>
-  <si>
     <t>3x Execute</t>
   </si>
   <si>
@@ -1137,6 +1134,9 @@
   </si>
   <si>
     <t>T1091.000.V1.cpp</t>
+  </si>
+  <si>
+    <t>Summary</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1546,7 @@
   <dimension ref="A1:P131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,8 +1557,8 @@
     <col min="4" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="16.28515625" customWidth="1"/>
     <col min="17" max="17" width="5.28515625" customWidth="1"/>
   </cols>
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>278</v>
       </c>
       <c r="G1" t="s">
         <v>71</v>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -1588,7 +1588,7 @@
         <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -1606,1233 +1606,1221 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" t="s">
         <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" s="4">
         <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7">
-        <f>C7+D7*P2</f>
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8">
-        <f>C8+D8*P2</f>
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9">
-        <f>C9+D9*P2</f>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
         <v>72</v>
       </c>
       <c r="H10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="G12" t="s">
         <v>72</v>
       </c>
       <c r="H12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="F14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H14" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="4">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" t="s">
         <v>224</v>
-      </c>
-      <c r="B15" t="s">
-        <v>225</v>
       </c>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" t="s">
         <v>100</v>
       </c>
-      <c r="F16" t="s">
-        <v>102</v>
-      </c>
-      <c r="G16" t="s">
-        <v>101</v>
-      </c>
       <c r="H16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I16" s="4">
         <v>1</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G18" t="s">
-        <v>106</v>
-      </c>
-      <c r="H18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>108</v>
+      </c>
+      <c r="H20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="F20" t="s">
-        <v>111</v>
-      </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="G23" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P24" s="1"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P27" s="1"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" t="s">
+        <v>116</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="G29" t="s">
-        <v>96</v>
-      </c>
-      <c r="H29" t="s">
-        <v>117</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="P29" s="1"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P30" s="1"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P31" s="1"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" s="9">
+        <v>1</v>
+      </c>
+      <c r="J32" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="G32" t="s">
-        <v>121</v>
-      </c>
-      <c r="H32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I32" s="9">
-        <v>1</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I34" s="4">
         <v>1</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P34" s="1"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P35" s="1"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P36" s="1"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" t="s">
+        <v>215</v>
+      </c>
+      <c r="C37" t="s">
         <v>216</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>217</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>218</v>
-      </c>
-      <c r="E37" t="s">
-        <v>219</v>
       </c>
       <c r="P37" s="1"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P38" s="1"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P39" s="1"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" t="s">
         <v>126</v>
       </c>
-      <c r="G40" t="s">
-        <v>109</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="I40" s="4">
+        <v>1</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="I40" s="4">
-        <v>1</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="P40" s="1"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P41" s="1"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42" t="s">
         <v>130</v>
       </c>
-      <c r="G42" t="s">
-        <v>132</v>
-      </c>
-      <c r="H42" t="s">
-        <v>131</v>
-      </c>
       <c r="I42" s="4">
         <v>1</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P42" s="1"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P43" s="1"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P44" s="1"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>132</v>
+      </c>
+      <c r="G45" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" t="s">
         <v>133</v>
       </c>
-      <c r="G45" t="s">
-        <v>96</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="I45" s="4">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="I45" s="4">
-        <v>1</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="P45" s="1"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P46" s="1"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H47" t="s">
+        <v>137</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1</v>
+      </c>
+      <c r="J47" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="I47" s="4">
-        <v>1</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="P47" s="1"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B48" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P48" s="1"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B49" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P49" s="1"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H50" t="s">
+        <v>139</v>
+      </c>
+      <c r="I50" s="4">
+        <v>1</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="I50" s="4">
-        <v>1</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="P50" s="1"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P51" s="1"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P52" s="1"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>142</v>
+      </c>
+      <c r="G53" t="s">
+        <v>144</v>
+      </c>
+      <c r="H53" t="s">
         <v>143</v>
       </c>
-      <c r="G53" t="s">
-        <v>145</v>
-      </c>
-      <c r="H53" t="s">
-        <v>144</v>
-      </c>
       <c r="I53" s="4">
         <v>1</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P53" s="1"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P54" s="1"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B55" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P55" s="1"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="G56" t="s">
         <v>148</v>
       </c>
-      <c r="G56" t="s">
-        <v>149</v>
-      </c>
       <c r="H56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I56" s="4">
         <v>1</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P56" s="1"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B57" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P57" s="1"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="G58" t="s">
+        <v>148</v>
+      </c>
+      <c r="H58" t="s">
+        <v>146</v>
+      </c>
+      <c r="I58" s="4">
+        <v>1</v>
+      </c>
+      <c r="J58" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="G58" t="s">
-        <v>149</v>
-      </c>
-      <c r="H58" t="s">
-        <v>147</v>
-      </c>
-      <c r="I58" s="4">
-        <v>1</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="P58" s="1"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="P59" s="1"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>151</v>
+      </c>
+      <c r="G60" t="s">
+        <v>154</v>
+      </c>
+      <c r="H60" t="s">
+        <v>153</v>
+      </c>
+      <c r="I60" s="4">
+        <v>1</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="G60" t="s">
-        <v>155</v>
-      </c>
-      <c r="H60" t="s">
-        <v>154</v>
-      </c>
-      <c r="I60" s="4">
-        <v>1</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="P60" s="1"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P61" s="1"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P62" s="1"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I63" s="4">
         <v>1</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P63" s="1"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P64" s="1"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P65" s="1"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B66" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P66" s="1"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P67" s="1"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F68" t="s">
         <v>56</v>
       </c>
       <c r="G68" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H68" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I68" s="4">
         <v>1</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P68" s="1"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B69" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P69" s="1"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F70" t="s">
         <v>56</v>
       </c>
       <c r="G70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H70" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I70" s="4">
         <v>1</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P70" s="1"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B71" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P71" s="1"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F72" t="s">
         <v>56</v>
       </c>
       <c r="G72" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I72" s="4">
         <v>1</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P72" s="1"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B73" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P73" s="1"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P74" s="1"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B75" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P75" s="1"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B76" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P76" s="1"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B77" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P77" s="1"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P78" s="1"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H79" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I79" s="4">
         <v>1</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P79" s="1"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B80" t="s">
+        <v>255</v>
+      </c>
+      <c r="C80" t="s">
         <v>256</v>
-      </c>
-      <c r="C80" t="s">
-        <v>257</v>
       </c>
       <c r="P80" s="1"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>167</v>
+      </c>
+      <c r="F81" t="s">
+        <v>170</v>
+      </c>
+      <c r="G81" t="s">
+        <v>148</v>
+      </c>
+      <c r="H81" t="s">
+        <v>169</v>
+      </c>
+      <c r="I81" s="4">
+        <v>1</v>
+      </c>
+      <c r="J81" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="F81" t="s">
-        <v>171</v>
-      </c>
-      <c r="G81" t="s">
-        <v>149</v>
-      </c>
-      <c r="H81" t="s">
-        <v>170</v>
-      </c>
-      <c r="I81" s="4">
-        <v>1</v>
-      </c>
-      <c r="J81" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="P81" s="1"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P82" s="1"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P83" s="1"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B84" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="P84" s="1"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="P85" s="1"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P86" s="1"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P87" s="1"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>171</v>
+      </c>
+      <c r="G88" t="s">
+        <v>148</v>
+      </c>
+      <c r="H88" t="s">
+        <v>173</v>
+      </c>
+      <c r="I88" s="4">
+        <v>1</v>
+      </c>
+      <c r="J88" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="G88" t="s">
-        <v>149</v>
-      </c>
-      <c r="H88" t="s">
-        <v>174</v>
-      </c>
-      <c r="I88" s="4">
-        <v>1</v>
-      </c>
-      <c r="J88" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="P88" s="1"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P89" s="1"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P90" s="1"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>174</v>
+      </c>
+      <c r="G91" t="s">
+        <v>148</v>
+      </c>
+      <c r="H91" t="s">
+        <v>176</v>
+      </c>
+      <c r="I91" s="4">
+        <v>1</v>
+      </c>
+      <c r="J91" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="G91" t="s">
-        <v>149</v>
-      </c>
-      <c r="H91" t="s">
-        <v>177</v>
-      </c>
-      <c r="I91" s="4">
-        <v>1</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="P91" s="1"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P92" s="1"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B93" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P93" s="1"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>177</v>
+      </c>
+      <c r="G94" t="s">
+        <v>148</v>
+      </c>
+      <c r="H94" t="s">
+        <v>179</v>
+      </c>
+      <c r="I94" s="4">
+        <v>1</v>
+      </c>
+      <c r="J94" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="G94" t="s">
-        <v>149</v>
-      </c>
-      <c r="H94" t="s">
-        <v>180</v>
-      </c>
-      <c r="I94" s="4">
-        <v>1</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="P94" s="1"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B95" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P95" s="1"/>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>181</v>
+      </c>
+      <c r="F96" t="s">
         <v>182</v>
       </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
+        <v>95</v>
+      </c>
+      <c r="H96" t="s">
         <v>183</v>
       </c>
-      <c r="G96" t="s">
-        <v>96</v>
-      </c>
-      <c r="H96" t="s">
-        <v>184</v>
-      </c>
       <c r="I96" s="4">
         <v>1</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P96" s="1"/>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B97" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P97" s="1"/>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B98" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P98" s="1"/>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P99" s="1"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F100" t="s">
+        <v>184</v>
+      </c>
+      <c r="G100" t="s">
+        <v>108</v>
+      </c>
+      <c r="H100" t="s">
         <v>186</v>
       </c>
-      <c r="F100" t="s">
-        <v>185</v>
-      </c>
-      <c r="G100" t="s">
-        <v>109</v>
-      </c>
-      <c r="H100" t="s">
+      <c r="I100" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J100" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="I100" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="P100" s="1"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F101" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I101" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P101" s="1"/>
     </row>
@@ -2842,10 +2830,10 @@
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I102" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P102" s="1"/>
     </row>
@@ -2855,51 +2843,51 @@
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I103" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P103" s="1"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E104">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F104" t="s">
+        <v>193</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J104" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="I104" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="P104" s="1"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B105" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E105">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P105" s="1"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -2915,16 +2903,16 @@
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I106" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P106" s="1"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -2940,13 +2928,13 @@
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I107" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J107" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P107" s="1"/>
     </row>
@@ -2956,16 +2944,16 @@
         <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I108" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P108" s="1"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -2978,13 +2966,13 @@
         <v>1</v>
       </c>
       <c r="F109" t="s">
+        <v>203</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J109" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="I109" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="P109" s="1"/>
     </row>
@@ -2994,34 +2982,34 @@
         <v>0</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P110" s="1"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P111" s="1"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F112" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I112" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P112" s="1"/>
     </row>
     <row r="113" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F113" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I113" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P113" s="1"/>
     </row>
@@ -3298,7 +3286,7 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3444,7 +3432,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19">
         <f>COUNTA(D2:D17)</f>
@@ -3504,10 +3492,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D26" t="s">
         <v>275</v>
-      </c>
-      <c r="D26" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3542,7 +3530,7 @@
         <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F30" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
added command to generate sources for clean command
</commit_message>
<xml_diff>
--- a/MiTRE/MitreOperations.xlsx
+++ b/MiTRE/MitreOperations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AssistantsTesterGithub\MiTRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63F12B1-2219-49D1-9EF1-CA44A9A04C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5EEA9CD8-FF95-4D5F-B829-DD4EBD04DBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ImplementedOperations" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="289">
   <si>
     <t>Operation</t>
   </si>
@@ -1137,6 +1137,36 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Clean1003.001</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>"procdump -ma lsass.exe lsassdump"</t>
+  </si>
+  <si>
+    <t>"rundll32.exe C:\\Windows\\System32\\comsvcs.dll Mini_Dump PID lsass.dmp full"</t>
+  </si>
+  <si>
+    <t>Clean1562.004</t>
+  </si>
+  <si>
+    <t>"netsh advfirewall firewell delete rule name=\"My Rule\""</t>
+  </si>
+  <si>
+    <t>"netsh advfirewall firewall badd rule name=\"some_rule\" dir=in action=allow protocol=TCP localport=1256 program=\"C:\\x.exe\" description=\"xxx\" enable=yes"</t>
+  </si>
+  <si>
+    <t>Clean1136.001</t>
+  </si>
+  <si>
+    <t>"/c net user /ad test"</t>
+  </si>
+  <si>
+    <t>"net user add abc"</t>
   </si>
 </sst>
 </file>
@@ -1545,13 +1575,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4627B1-CCD6-45EF-95C0-ACBE31171D5D}">
   <dimension ref="A1:P131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="5" width="12.5703125" customWidth="1"/>
@@ -2795,200 +2825,104 @@
       <c r="P99" s="1"/>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="F100" t="s">
-        <v>184</v>
-      </c>
-      <c r="G100" t="s">
-        <v>108</v>
-      </c>
-      <c r="H100" t="s">
-        <v>186</v>
-      </c>
-      <c r="I100" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J100" s="2" t="s">
-        <v>187</v>
+      <c r="A100" t="s">
+        <v>279</v>
       </c>
       <c r="P100" s="1"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F101" t="s">
-        <v>189</v>
-      </c>
-      <c r="I101" s="5" t="s">
-        <v>188</v>
+      <c r="A101" t="s">
+        <v>280</v>
+      </c>
+      <c r="B101" t="s">
+        <v>281</v>
       </c>
       <c r="P101" s="1"/>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E102">
-        <f>C102+D102*P32</f>
-        <v>0</v>
-      </c>
-      <c r="F102" t="s">
-        <v>190</v>
-      </c>
-      <c r="I102" s="5" t="s">
-        <v>188</v>
+      <c r="A102" t="s">
+        <v>280</v>
+      </c>
+      <c r="B102" t="s">
+        <v>282</v>
       </c>
       <c r="P102" s="1"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E103">
-        <f t="shared" ref="E103:E110" si="0">C103+D103*P34</f>
-        <v>0</v>
-      </c>
-      <c r="F103" t="s">
-        <v>191</v>
-      </c>
-      <c r="I103" s="5" t="s">
-        <v>188</v>
+      <c r="A103" t="s">
+        <v>283</v>
       </c>
       <c r="P103" s="1"/>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>192</v>
-      </c>
-      <c r="E104">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F104" t="s">
-        <v>193</v>
-      </c>
-      <c r="I104" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>194</v>
+        <v>280</v>
+      </c>
+      <c r="B104" t="s">
+        <v>285</v>
       </c>
       <c r="P104" s="1"/>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>195</v>
+        <v>280</v>
       </c>
       <c r="B105" t="s">
-        <v>188</v>
-      </c>
-      <c r="E105">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I105" s="5" t="s">
-        <v>188</v>
+        <v>284</v>
       </c>
       <c r="P105" s="1"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>197</v>
-      </c>
-      <c r="B106">
-        <v>0</v>
-      </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
-      <c r="E106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F106" t="s">
-        <v>196</v>
-      </c>
-      <c r="I106" s="5" t="s">
-        <v>188</v>
+        <v>286</v>
       </c>
       <c r="P106" s="1"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>199</v>
-      </c>
-      <c r="B107">
-        <v>0</v>
-      </c>
-      <c r="C107">
-        <v>1</v>
-      </c>
-      <c r="D107">
-        <v>1</v>
-      </c>
-      <c r="E107">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F107" t="s">
-        <v>200</v>
-      </c>
-      <c r="I107" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J107" s="2" t="s">
-        <v>198</v>
+        <v>280</v>
+      </c>
+      <c r="B107" t="s">
+        <v>287</v>
       </c>
       <c r="P107" s="1"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E108">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F108" t="s">
-        <v>201</v>
-      </c>
-      <c r="I108" s="5" t="s">
-        <v>188</v>
+      <c r="A108" t="s">
+        <v>280</v>
+      </c>
+      <c r="B108" t="s">
+        <v>288</v>
       </c>
       <c r="P108" s="1"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>202</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="E109">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
-        <v>203</v>
-      </c>
-      <c r="I109" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J109" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="P109" s="1"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E110">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A110" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F110" t="s">
+        <v>184</v>
+      </c>
+      <c r="G110" t="s">
+        <v>108</v>
+      </c>
+      <c r="H110" t="s">
+        <v>186</v>
       </c>
       <c r="I110" s="5" t="s">
         <v>188</v>
       </c>
+      <c r="J110" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="P110" s="1"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="I111" s="5" t="s">
         <v>188</v>
@@ -2996,66 +2930,207 @@
       <c r="P111" s="1"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <f>C112+D112*P32</f>
+        <v>0</v>
+      </c>
       <c r="F112" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="I112" s="5" t="s">
         <v>188</v>
       </c>
       <c r="P112" s="1"/>
     </row>
-    <row r="113" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F113" s="2" t="s">
-        <v>208</v>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <f>C113+D113*P34</f>
+        <v>0</v>
+      </c>
+      <c r="F113" t="s">
+        <v>191</v>
       </c>
       <c r="I113" s="5" t="s">
         <v>188</v>
       </c>
       <c r="P113" s="1"/>
     </row>
-    <row r="114" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>192</v>
+      </c>
+      <c r="E114">
+        <f>C114+D114*P35</f>
+        <v>0</v>
+      </c>
+      <c r="F114" t="s">
+        <v>193</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="P114" s="1"/>
     </row>
-    <row r="115" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>195</v>
+      </c>
+      <c r="B115" t="s">
+        <v>188</v>
+      </c>
+      <c r="E115">
+        <f>C115+D115*P36</f>
+        <v>0</v>
+      </c>
+      <c r="I115" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P115" s="1"/>
     </row>
-    <row r="116" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>197</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <f>C116+D116*P37</f>
+        <v>0</v>
+      </c>
+      <c r="F116" t="s">
+        <v>196</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P116" s="1"/>
     </row>
-    <row r="117" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>199</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <f>C117+D117*P38</f>
+        <v>1</v>
+      </c>
+      <c r="F117" t="s">
+        <v>200</v>
+      </c>
+      <c r="I117" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="P117" s="1"/>
     </row>
-    <row r="118" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <f>C118+D118*P39</f>
+        <v>0</v>
+      </c>
+      <c r="F118" t="s">
+        <v>201</v>
+      </c>
+      <c r="I118" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P118" s="1"/>
     </row>
-    <row r="119" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>202</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <f>C119+D119*P40</f>
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>203</v>
+      </c>
+      <c r="I119" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="P119" s="1"/>
     </row>
-    <row r="120" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <f>C120+D120*P41</f>
+        <v>0</v>
+      </c>
+      <c r="I120" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P120" s="1"/>
     </row>
-    <row r="121" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
+        <v>206</v>
+      </c>
+      <c r="I121" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P121" s="1"/>
     </row>
-    <row r="122" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
+        <v>207</v>
+      </c>
+      <c r="I122" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P122" s="1"/>
     </row>
-    <row r="123" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F123" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I123" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="P123" s="1"/>
     </row>
-    <row r="124" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P124" s="1"/>
     </row>
-    <row r="125" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P125" s="1"/>
     </row>
-    <row r="126" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P126" s="1"/>
     </row>
-    <row r="127" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P127" s="1"/>
     </row>
-    <row r="128" spans="6:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P128" s="1"/>
     </row>
     <row r="129" spans="16:16" x14ac:dyDescent="0.25">
@@ -3101,11 +3176,11 @@
     <hyperlink ref="J91" r:id="rId29" xr:uid="{D5E29CDB-ED2B-4A96-AE32-8141A2955370}"/>
     <hyperlink ref="J94" r:id="rId30" xr:uid="{8F4B9E06-3CED-47F1-B93F-1207A48E16B5}"/>
     <hyperlink ref="J96" r:id="rId31" xr:uid="{98E8F283-8F69-4CC5-A4FF-CB5301CF9F96}"/>
-    <hyperlink ref="J104" r:id="rId32" xr:uid="{439D2314-9B22-415F-A5A1-3563D4642932}"/>
-    <hyperlink ref="J100" r:id="rId33" xr:uid="{8C102FE7-D93B-4BD9-A57B-C72DAD4EDBA2}"/>
-    <hyperlink ref="J107" r:id="rId34" xr:uid="{E62C70A8-FDB5-421A-AFA1-E3262C592104}"/>
-    <hyperlink ref="J109" r:id="rId35" xr:uid="{C2297CF9-E7ED-417B-968E-0AAE230EDB1A}"/>
-    <hyperlink ref="F113" r:id="rId36" xr:uid="{5E6A4597-E97E-48FB-96BA-F6F33955E589}"/>
+    <hyperlink ref="J114" r:id="rId32" xr:uid="{439D2314-9B22-415F-A5A1-3563D4642932}"/>
+    <hyperlink ref="J110" r:id="rId33" xr:uid="{8C102FE7-D93B-4BD9-A57B-C72DAD4EDBA2}"/>
+    <hyperlink ref="J117" r:id="rId34" xr:uid="{E62C70A8-FDB5-421A-AFA1-E3262C592104}"/>
+    <hyperlink ref="J119" r:id="rId35" xr:uid="{C2297CF9-E7ED-417B-968E-0AAE230EDB1A}"/>
+    <hyperlink ref="F123" r:id="rId36" xr:uid="{5E6A4597-E97E-48FB-96BA-F6F33955E589}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated first clean command
</commit_message>
<xml_diff>
--- a/MiTRE/MitreOperations.xlsx
+++ b/MiTRE/MitreOperations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\AssistantsTesterGithub\MiTRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5EEA9CD8-FF95-4D5F-B829-DD4EBD04DBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19491079-63BA-4C41-90D3-832F6F6233D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1145,9 +1145,6 @@
     <t>clean</t>
   </si>
   <si>
-    <t>"procdump -ma lsass.exe lsassdump"</t>
-  </si>
-  <si>
     <t>"rundll32.exe C:\\Windows\\System32\\comsvcs.dll Mini_Dump PID lsass.dmp full"</t>
   </si>
   <si>
@@ -1167,6 +1164,9 @@
   </si>
   <si>
     <t>"net user add abc"</t>
+  </si>
+  <si>
+    <t>"procdump ma lsass.exe lsassdump"</t>
   </si>
 </sst>
 </file>
@@ -1575,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA4627B1-CCD6-45EF-95C0-ACBE31171D5D}">
   <dimension ref="A1:P131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2835,7 +2835,7 @@
         <v>280</v>
       </c>
       <c r="B101" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="P101" s="1"/>
     </row>
@@ -2844,13 +2844,13 @@
         <v>280</v>
       </c>
       <c r="B102" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P102" s="1"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P103" s="1"/>
     </row>
@@ -2859,7 +2859,7 @@
         <v>280</v>
       </c>
       <c r="B104" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P104" s="1"/>
     </row>
@@ -2868,13 +2868,13 @@
         <v>280</v>
       </c>
       <c r="B105" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P105" s="1"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P106" s="1"/>
     </row>
@@ -2883,7 +2883,7 @@
         <v>280</v>
       </c>
       <c r="B107" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P107" s="1"/>
     </row>
@@ -2892,7 +2892,7 @@
         <v>280</v>
       </c>
       <c r="B108" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="P108" s="1"/>
     </row>
@@ -2944,7 +2944,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E113">
-        <f>C113+D113*P34</f>
+        <f t="shared" ref="E113:E120" si="0">C113+D113*P34</f>
         <v>0</v>
       </c>
       <c r="F113" t="s">
@@ -2960,7 +2960,7 @@
         <v>192</v>
       </c>
       <c r="E114">
-        <f>C114+D114*P35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F114" t="s">
@@ -2982,7 +2982,7 @@
         <v>188</v>
       </c>
       <c r="E115">
-        <f>C115+D115*P36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I115" s="5" t="s">
@@ -3004,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="E116">
-        <f>C116+D116*P37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F116" t="s">
@@ -3029,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="E117">
-        <f>C117+D117*P38</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F117" t="s">
@@ -3045,7 +3045,7 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E118">
-        <f>C118+D118*P39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F118" t="s">
@@ -3067,7 +3067,7 @@
         <v>0</v>
       </c>
       <c r="E119">
-        <f>C119+D119*P40</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F119" t="s">
@@ -3083,7 +3083,7 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E120">
-        <f>C120+D120*P41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I120" s="5" t="s">

</xml_diff>